<commit_message>
TCO hesaplamalar, kredi ve hurda modelleri eklendi
</commit_message>
<xml_diff>
--- a/r_input/esneklik.xlsx
+++ b/r_input/esneklik.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Desktop\eski bilgisayarlar\ICCT harddisk\ICCT blgisayar\Turkey- Tax System\R\r_input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Desktop\eski bilgisayarlar\ICCT harddisk\ICCT blgisayar\Turkey- Tax System\R\TR_tax_system\r_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3173F62-6B3F-48CA-8B9D-DB43663A1E81}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E52EB3B-40D7-4299-80F9-8A866214432D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="esneklik" sheetId="2" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="36">
   <si>
     <t>segment_text</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>large_suv</t>
+  </si>
+  <si>
+    <t>TCO-talep esnekligi</t>
   </si>
 </sst>
 </file>
@@ -504,10 +507,10 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,7 +531,7 @@
         <v>27</v>
       </c>
       <c r="B2">
-        <v>-1.66</v>
+        <v>-2.8</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -536,7 +539,15 @@
         <v>28</v>
       </c>
       <c r="B3">
-        <v>0.82</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4">
+        <v>-2.8</v>
       </c>
     </row>
   </sheetData>
@@ -683,7 +694,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4B67146-0022-4AC7-8AE3-42B7EEC97CCE}">
   <dimension ref="A1:L12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
LCV icin OTV,hurda ve kredi eklendi
</commit_message>
<xml_diff>
--- a/r_input/esneklik.xlsx
+++ b/r_input/esneklik.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Desktop\eski bilgisayarlar\ICCT harddisk\ICCT blgisayar\Turkey- Tax System\R\TR_tax_system\r_input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E52EB3B-40D7-4299-80F9-8A866214432D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9907837A-C304-4B23-9BC8-78668CEBEBC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="esneklik" sheetId="2" r:id="rId1"/>
-    <sheet name="segments" sheetId="1" r:id="rId2"/>
-    <sheet name="kleit_segment_elasticity" sheetId="3" r:id="rId3"/>
+    <sheet name="esneklik (binek)" sheetId="2" r:id="rId1"/>
+    <sheet name="LCV esneklik" sheetId="4" r:id="rId2"/>
+    <sheet name="segments" sheetId="1" r:id="rId3"/>
+    <sheet name="kleit_segment_elasticity" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="37">
   <si>
     <t>segment_text</t>
   </si>
@@ -135,6 +136,9 @@
   </si>
   <si>
     <t>TCO-talep esnekligi</t>
+  </si>
+  <si>
+    <t>LCV  fiyat-talep esnekligi</t>
   </si>
 </sst>
 </file>
@@ -509,8 +513,8 @@
   </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -557,6 +561,40 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{960446CC-1FDF-4B3B-AB5B-EE0CFAF15CAB}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2">
+        <v>-2.8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C11"/>
   <sheetViews>
@@ -690,7 +728,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4B67146-0022-4AC7-8AE3-42B7EEC97CCE}">
   <dimension ref="A1:L12"/>
   <sheetViews>

</xml_diff>